<commit_message>
Pass 5V module AutoTrim
@shJoshDing
todo:
load config data, and update to control box
</commit_message>
<xml_diff>
--- a/Programming Discription/软件修改说明文件.xlsx
+++ b/Programming Discription/软件修改说明文件.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>软件修改说明 20150126A</t>
   </si>
@@ -140,6 +140,9 @@
   </si>
   <si>
     <t>细调Offset使用的寄存器数据位是：</t>
+  </si>
+  <si>
+    <t>load config之后， Reg1-4的显示要跟着变化；</t>
   </si>
 </sst>
 </file>
@@ -147,7 +150,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="[DBNum1][$-804]General"/>
+    <numFmt numFmtId="164" formatCode="[DBNum1][$-804]General"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -196,21 +199,21 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="13" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="13" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -569,10 +572,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R34"/>
+  <dimension ref="A1:R37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33:F34"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -846,6 +849,11 @@
         <v>39</v>
       </c>
     </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Modify some behavior of control box
@shJoshDing
load config之后， Reg1-4的显示更新;
PreTrim Tab增加一个choosen Gain显示如同AutoTrim Tab;
EngTab和PreTrim Tab的寄存器编辑框，任一的值变化了，需要同步；
</commit_message>
<xml_diff>
--- a/Programming Discription/软件修改说明文件.xlsx
+++ b/Programming Discription/软件修改说明文件.xlsx
@@ -133,9 +133,6 @@
     <t>细调Offset使用的寄存器数据位是：</t>
   </si>
   <si>
-    <t>load config之后， Reg1-4的显示要跟着变化；</t>
-  </si>
-  <si>
     <t>PreTrim Tab增加一个choosen Gain显示如同AutoTrim Tab；</t>
   </si>
   <si>
@@ -152,6 +149,9 @@
   </si>
   <si>
     <t>open</t>
+  </si>
+  <si>
+    <t>load config之后， Reg1-4的显示更新；</t>
   </si>
 </sst>
 </file>
@@ -229,45 +229,11 @@
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -625,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -640,7 +606,7 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -648,7 +614,7 @@
         <v>35</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>36</v>
@@ -891,7 +857,7 @@
         <v>1</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>37</v>
@@ -902,7 +868,7 @@
         <v>2</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>38</v>
@@ -919,10 +885,10 @@
         <v>1</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -930,10 +896,10 @@
         <v>2</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -941,10 +907,10 @@
         <v>3</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -952,15 +918,15 @@
         <v>4</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>$D$1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
V3.0.3 RC, under test
@shJoshDing
EngT增加一个ADCout按钮和显示，用于手动采集510out，Mout，Current 等；
AutoTrim流程调整，先写PreSet code,在采集Vout@IP和Vout@0A，之后再计算trim code；
</commit_message>
<xml_diff>
--- a/Programming Discription/软件修改说明文件.xlsx
+++ b/Programming Discription/软件修改说明文件.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
   <si>
     <t>软件修改说明 20150126A</t>
   </si>
@@ -152,6 +152,15 @@
   </si>
   <si>
     <t>load config之后， Reg1-4的显示更新；</t>
+  </si>
+  <si>
+    <t>EngT增加一个ADCout按钮和显示，用于手动采集510out，Mout，Current 等；</t>
+  </si>
+  <si>
+    <t>AutoTrim流程调整，先写PreSet code,在采集Vout@IP和Vout@0A，之后再计算trim code；</t>
+  </si>
+  <si>
+    <t>v3.0.3</t>
   </si>
 </sst>
 </file>
@@ -589,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R40"/>
+  <dimension ref="A1:R45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -924,6 +933,42 @@
         <v>41</v>
       </c>
     </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C41" s="1"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C42" s="1"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>1</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>2</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">

</xml_diff>